<commit_message>
Preliminary analysis done on tableu
</commit_message>
<xml_diff>
--- a/Personal data viz.xlsx
+++ b/Personal data viz.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="108">
   <si>
     <t>Year</t>
   </si>
@@ -818,7 +818,7 @@
   <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1536,7 +1536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:14">
       <c r="A17">
         <v>2008</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:14">
       <c r="A18">
         <v>2008</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:14">
       <c r="A19">
         <v>2008</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:14">
       <c r="A20">
         <v>2009</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:14">
       <c r="A21">
         <v>2009</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:14">
       <c r="A22">
         <v>2009</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:14">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:14">
       <c r="A24">
         <v>2010</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:14">
       <c r="A25">
         <v>2010</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:14">
       <c r="A26">
         <v>2010</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:14">
       <c r="A27">
         <v>2010</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:14">
       <c r="A28">
         <v>2011</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:14">
       <c r="A29">
         <v>2011</v>
       </c>
@@ -2105,11 +2105,8 @@
       <c r="N29">
         <v>4</v>
       </c>
-      <c r="O29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30">
         <v>2011</v>
       </c>
@@ -2153,7 +2150,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:14">
       <c r="A31">
         <v>2011</v>
       </c>
@@ -2197,7 +2194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:14">
       <c r="A32">
         <v>2011</v>
       </c>

</xml_diff>